<commit_message>
updated all files. created 4 visualizations. Still need finalizations
</commit_message>
<xml_diff>
--- a/Arrivals2016_by_county.xlsx
+++ b/Arrivals2016_by_county.xlsx
@@ -1,141 +1,146 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="123820"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayat Amin\Desktop\SDRefugees\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
-    <sheet name="page 1" sheetId="1" r:id="rId3"/>
-    <sheet name="page 2" sheetId="2" r:id="rId4"/>
+    <sheet name="page 1" sheetId="1" r:id="rId1"/>
+    <sheet name="page 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38" count="110">
-  <si>
-    <t xml:space="preserve">COUNTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oct-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nov-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feb-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mar-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apr-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jun-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jul-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aug-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alameda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contra Costa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Dorado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fresno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los Angeles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monterey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riverside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sacramento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Bernardino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Diego</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Francisco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Joaquin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santa Clara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stanislaus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yolo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,338</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,462</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>Oct-15</t>
+  </si>
+  <si>
+    <t>Nov-15</t>
+  </si>
+  <si>
+    <t>Dec-15</t>
+  </si>
+  <si>
+    <t>Jan-16</t>
+  </si>
+  <si>
+    <t>Feb-16</t>
+  </si>
+  <si>
+    <t>Mar-16</t>
+  </si>
+  <si>
+    <t>Apr-16</t>
+  </si>
+  <si>
+    <t>May-16</t>
+  </si>
+  <si>
+    <t>Jun-16</t>
+  </si>
+  <si>
+    <t>Jul-16</t>
+  </si>
+  <si>
+    <t>Aug-16</t>
+  </si>
+  <si>
+    <t>Alameda</t>
+  </si>
+  <si>
+    <t>Contra Costa</t>
+  </si>
+  <si>
+    <t>El Dorado</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Fresno</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Monterey</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Placer</t>
+  </si>
+  <si>
+    <t>Riverside</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>San Bernardino</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>San Joaquin</t>
+  </si>
+  <si>
+    <t>Santa Clara</t>
+  </si>
+  <si>
+    <t>Solano</t>
+  </si>
+  <si>
+    <t>Stanislaus</t>
+  </si>
+  <si>
+    <t>Ventura</t>
+  </si>
+  <si>
+    <t>Yolo</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>2,010</t>
+  </si>
+  <si>
+    <t>1,096</t>
+  </si>
+  <si>
+    <t>2,338</t>
+  </si>
+  <si>
+    <t>6,462</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -144,36 +149,32 @@
       <charset val="204"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="0"/>
+    </font>
+    <font>
       <i/>
-      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="0"/>
-      <i/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="0"/>
-      <b/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -212,43 +213,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyAlignment="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyAlignment="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyAlignment="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyAlignment="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyAlignment="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyAlignment="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyAlignment="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyAlignment="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyAlignment="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyAlignment="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyAlignment="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -257,6 +275,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -303,7 +329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,9 +361,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,6 +396,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,20 +431,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:shade val="40000"/>
+                <a:satMod val="155000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="65000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:shade val="85000"/>
+                <a:satMod val="155000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:shade val="95000"/>
+                <a:satMod val="155000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -424,7 +452,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -439,7 +467,7 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="34925" cap="rnd" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -449,16 +477,16 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="50800" algn="tl" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="64000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="39000" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -467,22 +495,22 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="39000" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
           <a:scene3d>
-            <a:camera prst="orthographicFront">
+            <a:camera prst="orthographicFront" fov="0">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
             <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:lightRig>
           </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+          <a:sp3d prstMaterial="matte">
+            <a:bevelT h="22225"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -494,27 +522,24 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="50000"/>
+                <a:satMod val="155000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="75000"/>
+                <a:satMod val="155000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -544,67 +569,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.095238" customWidth="1"/>
-    <col min="2" max="2" width="10.285714" customWidth="1"/>
-    <col min="3" max="3" width="10.857143" customWidth="1"/>
-    <col min="4" max="4" width="10.666667" customWidth="1"/>
-    <col min="5" max="5" width="10.476190" customWidth="1"/>
-    <col min="6" max="6" width="10.476190" customWidth="1"/>
-    <col min="7" max="7" width="10.857143" customWidth="1"/>
-    <col min="8" max="8" width="10.476190" customWidth="1"/>
-    <col min="9" max="9" width="11.238095" customWidth="1"/>
-    <col min="10" max="10" width="10.857143" customWidth="1"/>
-    <col min="11" max="11" width="9.904762" customWidth="1"/>
-    <col min="12" max="12" width="10.857143" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="5" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="9.90625" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.1" customHeight="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:13" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="M1" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3">
@@ -640,9 +669,13 @@
       <c r="L2" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" ht="16.44" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="M2">
+        <f>SUM(B2:L2)</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="6">
@@ -678,74 +711,82 @@
       <c r="L3" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" ht="16.44" customHeight="1">
-      <c r="A4" t="s" s="2">
+      <c r="M3">
+        <f t="shared" ref="M3:M21" si="0">SUM(B3:L3)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s" s="4">
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="4">
         <v>3</v>
       </c>
-      <c r="H4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="L4" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" ht="16.44" customHeight="1">
-      <c r="A5" t="s" s="5">
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6">
         <v>6</v>
       </c>
-      <c r="C5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s" s="6">
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="6">
@@ -754,9 +795,13 @@
       <c r="L5" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" ht="16.44" customHeight="1">
-      <c r="A6" t="s" s="2">
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="3">
@@ -792,47 +837,55 @@
       <c r="L6" s="3">
         <v>360</v>
       </c>
-    </row>
-    <row r="7" ht="16.44" customHeight="1">
-      <c r="A7" t="s" s="5">
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="6">
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s" s="6">
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="6">
         <v>1</v>
       </c>
-      <c r="J7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="L7" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" ht="15.96" customHeight="1">
-      <c r="A8" t="s" s="2">
+      <c r="J7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="4">
@@ -868,12 +921,16 @@
       <c r="L8" s="4">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" ht="16.44" customHeight="1">
-      <c r="A9" t="s" s="5">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s" s="6">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="6">
@@ -891,7 +948,7 @@
       <c r="G9" s="6">
         <v>4</v>
       </c>
-      <c r="H9" t="s" s="6">
+      <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="6">
@@ -900,15 +957,19 @@
       <c r="J9" s="6">
         <v>2</v>
       </c>
-      <c r="K9" t="s" s="6">
+      <c r="K9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="L9" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" ht="16.44" customHeight="1">
-      <c r="A10" t="s" s="2">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="4">
@@ -920,10 +981,10 @@
       <c r="D10" s="4">
         <v>8</v>
       </c>
-      <c r="E10" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s" s="4">
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="4">
@@ -941,12 +1002,16 @@
       <c r="K10" s="4">
         <v>3</v>
       </c>
-      <c r="L10" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" ht="16.44" customHeight="1">
-      <c r="A11" t="s" s="5">
+      <c r="L10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="7">
@@ -982,9 +1047,13 @@
       <c r="L11" s="7">
         <v>240</v>
       </c>
-    </row>
-    <row r="12" ht="16.44" customHeight="1">
-      <c r="A12" t="s" s="2">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="4">
@@ -996,13 +1065,13 @@
       <c r="D12" s="4">
         <v>4</v>
       </c>
-      <c r="E12" t="s" s="4">
+      <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="4">
         <v>5</v>
       </c>
-      <c r="G12" t="s" s="4">
+      <c r="G12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="4">
@@ -1011,7 +1080,7 @@
       <c r="I12" s="4">
         <v>2</v>
       </c>
-      <c r="J12" t="s" s="4">
+      <c r="J12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="3">
@@ -1020,9 +1089,13 @@
       <c r="L12" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" ht="16.44" customHeight="1">
-      <c r="A13" t="s" s="5">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="7">
@@ -1058,59 +1131,67 @@
       <c r="L13" s="7">
         <v>620</v>
       </c>
-    </row>
-    <row r="14" ht="16.44" customHeight="1">
-      <c r="A14" t="s" s="2">
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="G14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="H14" t="s" s="4">
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="4">
         <v>3</v>
       </c>
-      <c r="J14" t="s" s="4">
+      <c r="J14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="4">
         <v>3</v>
       </c>
-      <c r="L14" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" ht="16.44" customHeight="1">
-      <c r="A15" t="s" s="5">
+      <c r="L14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s" s="6">
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="6">
@@ -1128,15 +1209,19 @@
       <c r="J15" s="6">
         <v>3</v>
       </c>
-      <c r="K15" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="L15" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" ht="16.44" customHeight="1">
-      <c r="A16" t="s" s="2">
+      <c r="K15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="4">
@@ -1172,24 +1257,28 @@
       <c r="L16" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" ht="16.44" customHeight="1">
-      <c r="A17" t="s" s="5">
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="F17" t="s" s="6">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="6">
@@ -1198,21 +1287,25 @@
       <c r="H17" s="6">
         <v>1</v>
       </c>
-      <c r="I17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="J17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="L17" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" ht="16.44" customHeight="1">
-      <c r="A18" t="s" s="2">
+      <c r="I17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3">
@@ -1227,7 +1320,7 @@
       <c r="E18" s="3">
         <v>13</v>
       </c>
-      <c r="F18" t="s" s="4">
+      <c r="F18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="4">
@@ -1248,33 +1341,37 @@
       <c r="L18" s="4">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" ht="16.44" customHeight="1">
-      <c r="A19" t="s" s="5">
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
       </c>
-      <c r="C19" t="s" s="6">
+      <c r="C19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="6">
         <v>6</v>
       </c>
-      <c r="E19" t="s" s="6">
+      <c r="E19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="6">
         <v>1</v>
       </c>
-      <c r="G19" t="s" s="6">
+      <c r="G19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="6">
         <v>3</v>
       </c>
-      <c r="I19" t="s" s="6">
+      <c r="I19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="6">
@@ -1286,15 +1383,19 @@
       <c r="L19" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" ht="16.44" customHeight="1">
-      <c r="A20" t="s" s="2">
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s" s="4">
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="4">
@@ -1303,30 +1404,34 @@
       <c r="E20" s="4">
         <v>7</v>
       </c>
-      <c r="F20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="G20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="H20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="I20" t="s" s="4">
+      <c r="F20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J20" s="4">
         <v>2</v>
       </c>
-      <c r="K20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="L20" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" ht="17.16" customHeight="1">
-      <c r="A21" t="s" s="1">
+      <c r="K20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1">
@@ -1359,8 +1464,12 @@
       <c r="K21" s="1">
         <v>764</v>
       </c>
-      <c r="L21" t="s" s="1">
-        <v>33</v>
+      <c r="L21" s="13">
+        <v>1425</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>6462</v>
       </c>
     </row>
   </sheetData>
@@ -1369,119 +1478,119 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.857143" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.1" customHeight="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>139</v>
       </c>
     </row>
-    <row r="3" ht="16.44" customHeight="1">
+    <row r="3" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>45</v>
       </c>
     </row>
-    <row r="4" ht="16.44" customHeight="1">
+    <row r="4" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="16.44" customHeight="1">
+    <row r="5" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>16</v>
       </c>
     </row>
-    <row r="6" ht="16.44" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" ht="16.44" customHeight="1">
+    <row r="6" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="15.96" customHeight="1">
+    <row r="8" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>148</v>
       </c>
     </row>
-    <row r="9" ht="16.44" customHeight="1">
+    <row r="9" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>41</v>
       </c>
     </row>
-    <row r="10" ht="16.44" customHeight="1">
+    <row r="10" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>36</v>
       </c>
     </row>
-    <row r="11" ht="16.44" customHeight="1">
-      <c r="A11" t="s" s="11">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" ht="16.44" customHeight="1">
+    <row r="11" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>50</v>
       </c>
     </row>
-    <row r="13" ht="16.44" customHeight="1">
-      <c r="A13" t="s" s="11">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" ht="16.44" customHeight="1">
+    <row r="13" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="15" ht="16.44" customHeight="1">
+    <row r="15" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>19</v>
       </c>
     </row>
-    <row r="16" ht="16.44" customHeight="1">
+    <row r="16" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>189</v>
       </c>
     </row>
-    <row r="17" ht="16.44" customHeight="1">
+    <row r="17" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="18" ht="16.44" customHeight="1">
+    <row r="18" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>290</v>
       </c>
     </row>
-    <row r="19" ht="16.44" customHeight="1">
+    <row r="19" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>17</v>
       </c>
     </row>
-    <row r="20" ht="16.44" customHeight="1">
+    <row r="20" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>12</v>
       </c>
     </row>
-    <row r="21" ht="17.16" customHeight="1">
-      <c r="A21" t="s" s="1">
-        <v>37</v>
+    <row r="21" spans="1:1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>